<commit_message>
Update DietaCronicaMexico.xlsx data file
Replaces the existing DietaCronicaMexico.xlsx file with a new version. The update likely includes revised or additional data for chronic diet analysis in Mexico.
</commit_message>
<xml_diff>
--- a/Backend/data/DietaCronicaMexico.xlsx
+++ b/Backend/data/DietaCronicaMexico.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://syngenta-my.sharepoint.com/personal/vinicius_camargo_syngenta_com/Documents/Área de Trabalho/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://syngenta-my.sharepoint.com/personal/vinicius_camargo_syngenta_com/Documents/Área de Trabalho/RiskWise_Frontend/Backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{53715433-5D7B-4B6D-AE97-745FC0A21E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE7FA96D-31FB-4B87-B740-DF1040974CDE}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="8_{53715433-5D7B-4B6D-AE97-745FC0A21E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C38192D7-6B28-4E3C-A43C-2DEAB615E973}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E0B61B8B-DA93-4BC2-B123-3E6FE07750BC}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{E0B61B8B-DA93-4BC2-B123-3E6FE07750BC}"/>
   </bookViews>
   <sheets>
     <sheet name="MX_chronic dietary" sheetId="1" r:id="rId1"/>
     <sheet name="Nombres IUPAC espanhol" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'MX_chronic dietary'!$D$7:$I$103</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'MX_chronic dietary'!$D$7:$I$111</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="209">
   <si>
     <t>ADI (mg/kg bw/day)</t>
   </si>
@@ -1807,6 +1807,87 @@
   </si>
   <si>
     <t>C (Kg/person/day)</t>
+  </si>
+  <si>
+    <t>Artichoke</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Alcachofa </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+  </si>
+  <si>
+    <t>Beet</t>
+  </si>
+  <si>
+    <t>Betabel 4</t>
+  </si>
+  <si>
+    <t>Cocoa</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Cacao </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+  </si>
+  <si>
+    <t>Plum</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ciruelo </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+  </si>
+  <si>
+    <t>Kiwi</t>
+  </si>
+  <si>
+    <t>Sapote Mammey</t>
+  </si>
+  <si>
+    <t>Mamey</t>
+  </si>
+  <si>
+    <t>Nectarine</t>
+  </si>
+  <si>
+    <t>Nectarino</t>
+  </si>
+  <si>
+    <t>Nopal²</t>
   </si>
 </sst>
 </file>
@@ -1817,7 +1898,7 @@
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1899,8 +1980,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1949,8 +2038,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -2178,11 +2273,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -2299,6 +2407,19 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2317,7 +2438,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -2613,28 +2734,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE9FD823-0127-4C95-94F5-6E3964FBBD64}">
-  <dimension ref="A1:M108"/>
+  <dimension ref="A1:M116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="108" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="8.7109375" style="1"/>
-    <col min="4" max="4" width="14.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="1" customWidth="1"/>
-    <col min="6" max="7" width="12.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" style="1"/>
-    <col min="11" max="11" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="21.5546875" style="1" customWidth="1"/>
+    <col min="2" max="3" width="8.6640625" style="1"/>
+    <col min="4" max="4" width="14.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="12.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" style="1"/>
+    <col min="11" max="11" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>134</v>
       </c>
@@ -2648,14 +2769,14 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="13"/>
       <c r="I2" s="42"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2669,7 +2790,7 @@
       <c r="G3" s="37"/>
       <c r="I3" s="43"/>
     </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -2678,7 +2799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -2690,11 +2811,11 @@
         <v>6</v>
       </c>
       <c r="I5" s="11">
-        <f>SUM(I8:I103)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <f>SUM(I8:I111)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D7" s="15" t="s">
         <v>4</v>
       </c>
@@ -2714,7 +2835,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D8" s="18" t="s">
         <v>59</v>
       </c>
@@ -2731,7 +2852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D9" s="18" t="s">
         <v>9</v>
       </c>
@@ -2746,7 +2867,7 @@
         <v>4.5999999999999999E-3</v>
       </c>
       <c r="I9" s="21">
-        <f t="shared" ref="I9:I72" si="0">IF(G9&lt;&gt;"-",G9*H9,F9*H9)</f>
+        <f t="shared" ref="I9:I78" si="0">IF(G9&lt;&gt;"-",G9*H9,F9*H9)</f>
         <v>0</v>
       </c>
       <c r="J9" s="7"/>
@@ -2754,7 +2875,7 @@
       <c r="L9" s="7"/>
       <c r="M9" s="9"/>
     </row>
-    <row r="10" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D10" s="18" t="s">
         <v>8</v>
       </c>
@@ -2777,19 +2898,19 @@
       <c r="L10" s="7"/>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D11" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="F11" s="19"/>
-      <c r="G11" s="33" t="s">
+    <row r="11" spans="1:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D11" s="44" t="s">
+        <v>195</v>
+      </c>
+      <c r="E11" s="45" t="s">
+        <v>196</v>
+      </c>
+      <c r="F11" s="45"/>
+      <c r="G11" s="20" t="s">
         <v>185</v>
       </c>
       <c r="H11" s="20">
-        <v>7.1399999999999996E-3</v>
+        <v>2.5999999999999998E-4</v>
       </c>
       <c r="I11" s="21">
         <f t="shared" si="0"/>
@@ -2800,19 +2921,19 @@
       <c r="L11" s="7"/>
       <c r="M11" s="9"/>
     </row>
-    <row r="12" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D12" s="18" t="s">
-        <v>51</v>
+        <v>157</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F12" s="19"/>
       <c r="G12" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H12" s="20">
-        <v>6.0000000000000002E-5</v>
+        <v>7.1399999999999996E-3</v>
       </c>
       <c r="I12" s="21">
         <f t="shared" si="0"/>
@@ -2823,38 +2944,40 @@
       <c r="L12" s="7"/>
       <c r="M12" s="9"/>
     </row>
-    <row r="13" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D13" s="18"/>
+    <row r="13" spans="1:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D13" s="18" t="s">
+        <v>51</v>
+      </c>
       <c r="E13" s="18" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F13" s="19"/>
       <c r="G13" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H13" s="20">
-        <v>4.2799999999999998E-2</v>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="I13" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J13" s="7"/>
+      <c r="J13" s="48"/>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
       <c r="M13" s="9"/>
     </row>
-    <row r="14" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D14" s="18"/>
       <c r="E14" s="18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F14" s="19"/>
       <c r="G14" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H14" s="20">
-        <v>2.0000000000000002E-5</v>
+        <v>4.2799999999999998E-2</v>
       </c>
       <c r="I14" s="21">
         <f t="shared" si="0"/>
@@ -2863,21 +2986,19 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
-      <c r="M14" s="10"/>
-    </row>
-    <row r="15" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D15" s="18" t="s">
-        <v>10</v>
-      </c>
+      <c r="M14" s="9"/>
+    </row>
+    <row r="15" spans="1:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D15" s="18"/>
       <c r="E15" s="18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F15" s="19"/>
       <c r="G15" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H15" s="20">
-        <v>1.0000000000000001E-5</v>
+        <v>2.0000000000000002E-5</v>
       </c>
       <c r="I15" s="21">
         <f t="shared" si="0"/>
@@ -2886,21 +3007,21 @@
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
-      <c r="M15" s="9"/>
-    </row>
-    <row r="16" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M15" s="10"/>
+    </row>
+    <row r="16" spans="1:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D16" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="F16" s="19"/>
       <c r="G16" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H16" s="20">
-        <v>4.1399999999999999E-2</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="I16" s="21">
         <f t="shared" si="0"/>
@@ -2911,19 +3032,19 @@
       <c r="L16" s="7"/>
       <c r="M16" s="9"/>
     </row>
-    <row r="17" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D17" s="18" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H17" s="20">
-        <v>1.0000000000000001E-5</v>
+        <v>4.1399999999999999E-2</v>
       </c>
       <c r="I17" s="21">
         <f t="shared" si="0"/>
@@ -2934,19 +3055,19 @@
       <c r="L17" s="7"/>
       <c r="M17" s="9"/>
     </row>
-    <row r="18" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D18" s="18" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="F18" s="19"/>
       <c r="G18" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H18" s="20">
-        <v>4.5999999999999999E-3</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="I18" s="21">
         <f t="shared" si="0"/>
@@ -2957,19 +3078,19 @@
       <c r="L18" s="7"/>
       <c r="M18" s="9"/>
     </row>
-    <row r="19" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D19" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="F19" s="19"/>
       <c r="G19" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H19" s="20">
-        <v>1.3639999999999999E-2</v>
+        <v>4.5999999999999999E-3</v>
       </c>
       <c r="I19" s="21">
         <f t="shared" si="0"/>
@@ -2980,19 +3101,19 @@
       <c r="L19" s="7"/>
       <c r="M19" s="9"/>
     </row>
-    <row r="20" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D20" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="33" t="s">
+    <row r="20" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D20" s="44" t="s">
+        <v>197</v>
+      </c>
+      <c r="E20" s="45" t="s">
+        <v>198</v>
+      </c>
+      <c r="F20" s="45"/>
+      <c r="G20" s="20" t="s">
         <v>185</v>
       </c>
       <c r="H20" s="20">
-        <v>4.1000000000000003E-3</v>
+        <v>9.3299999999999998E-3</v>
       </c>
       <c r="I20" s="21">
         <f t="shared" si="0"/>
@@ -3003,17 +3124,19 @@
       <c r="L20" s="7"/>
       <c r="M20" s="9"/>
     </row>
-    <row r="21" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D21" s="18"/>
+    <row r="21" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D21" s="18" t="s">
+        <v>13</v>
+      </c>
       <c r="E21" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F21" s="19"/>
       <c r="G21" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H21" s="20">
-        <v>1.17E-3</v>
+        <v>1.3639999999999999E-2</v>
       </c>
       <c r="I21" s="21">
         <f t="shared" si="0"/>
@@ -3024,17 +3147,19 @@
       <c r="L21" s="7"/>
       <c r="M21" s="9"/>
     </row>
-    <row r="22" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D22" s="18"/>
+    <row r="22" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D22" s="18" t="s">
+        <v>14</v>
+      </c>
       <c r="E22" s="18" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="F22" s="19"/>
       <c r="G22" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H22" s="20">
-        <v>1.3699999999999999E-3</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="I22" s="21">
         <f t="shared" si="0"/>
@@ -3045,17 +3170,19 @@
       <c r="L22" s="7"/>
       <c r="M22" s="9"/>
     </row>
-    <row r="23" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D23" s="18"/>
-      <c r="E23" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="F23" s="19"/>
-      <c r="G23" s="33" t="s">
+    <row r="23" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D23" s="46" t="s">
+        <v>199</v>
+      </c>
+      <c r="E23" s="45" t="s">
+        <v>200</v>
+      </c>
+      <c r="F23" s="45"/>
+      <c r="G23" s="20" t="s">
         <v>185</v>
       </c>
       <c r="H23" s="20">
-        <v>1.5900000000000001E-2</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="I23" s="21">
         <f t="shared" si="0"/>
@@ -3066,17 +3193,17 @@
       <c r="L23" s="7"/>
       <c r="M23" s="9"/>
     </row>
-    <row r="24" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D24" s="18"/>
       <c r="E24" s="18" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H24" s="20">
-        <v>3.3700000000000001E-2</v>
+        <v>1.17E-3</v>
       </c>
       <c r="I24" s="21">
         <f t="shared" si="0"/>
@@ -3087,19 +3214,17 @@
       <c r="L24" s="7"/>
       <c r="M24" s="9"/>
     </row>
-    <row r="25" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D25" s="18" t="s">
-        <v>15</v>
-      </c>
+    <row r="25" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D25" s="18"/>
       <c r="E25" s="18" t="s">
-        <v>139</v>
+        <v>96</v>
       </c>
       <c r="F25" s="19"/>
       <c r="G25" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H25" s="20">
-        <v>1.779E-2</v>
+        <v>1.3699999999999999E-3</v>
       </c>
       <c r="I25" s="21">
         <f t="shared" si="0"/>
@@ -3110,17 +3235,17 @@
       <c r="L25" s="7"/>
       <c r="M25" s="9"/>
     </row>
-    <row r="26" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D26" s="18"/>
       <c r="E26" s="18" t="s">
-        <v>138</v>
+        <v>107</v>
       </c>
       <c r="F26" s="19"/>
       <c r="G26" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H26" s="20">
-        <v>2.9E-4</v>
+        <v>1.5900000000000001E-2</v>
       </c>
       <c r="I26" s="21">
         <f t="shared" si="0"/>
@@ -3131,17 +3256,17 @@
       <c r="L26" s="7"/>
       <c r="M26" s="9"/>
     </row>
-    <row r="27" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D27" s="18"/>
       <c r="E27" s="18" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="F27" s="19"/>
       <c r="G27" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H27" s="20">
-        <v>9.0000000000000006E-5</v>
+        <v>3.3700000000000001E-2</v>
       </c>
       <c r="I27" s="21">
         <f t="shared" si="0"/>
@@ -3152,42 +3277,40 @@
       <c r="L27" s="7"/>
       <c r="M27" s="9"/>
     </row>
-    <row r="28" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D28" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="F28" s="19"/>
       <c r="G28" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H28" s="20">
-        <v>1.8000000000000001E-4</v>
+        <v>1.779E-2</v>
       </c>
       <c r="I28" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J28" s="7"/>
-      <c r="K28" s="34"/>
+      <c r="K28" s="7"/>
       <c r="L28" s="7"/>
       <c r="M28" s="9"/>
     </row>
-    <row r="29" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D29" s="18" t="s">
-        <v>17</v>
-      </c>
+    <row r="29" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D29" s="18"/>
       <c r="E29" s="18" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="F29" s="19"/>
       <c r="G29" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H29" s="20">
-        <v>2.47E-2</v>
+        <v>2.9E-4</v>
       </c>
       <c r="I29" s="21">
         <f t="shared" si="0"/>
@@ -3198,19 +3321,17 @@
       <c r="L29" s="7"/>
       <c r="M29" s="9"/>
     </row>
-    <row r="30" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D30" s="18" t="s">
-        <v>18</v>
-      </c>
+    <row r="30" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D30" s="18"/>
       <c r="E30" s="18" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F30" s="19"/>
       <c r="G30" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H30" s="20">
-        <v>5.9999999999999995E-4</v>
+        <v>9.0000000000000006E-5</v>
       </c>
       <c r="I30" s="21">
         <f t="shared" si="0"/>
@@ -3221,41 +3342,42 @@
       <c r="L30" s="7"/>
       <c r="M30" s="9"/>
     </row>
-    <row r="31" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D31" s="18" t="s">
-        <v>158</v>
+        <v>16</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F31" s="19"/>
       <c r="G31" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H31" s="20">
-        <v>3.0000000000000001E-5</v>
+        <v>1.8000000000000001E-4</v>
       </c>
       <c r="I31" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
+      <c r="K31" s="34"/>
       <c r="L31" s="7"/>
       <c r="M31" s="9"/>
     </row>
-    <row r="32" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D32" s="18"/>
-      <c r="E32" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="F32" s="28"/>
+    <row r="32" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D32" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="F32" s="19"/>
       <c r="G32" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="H32" s="29">
-        <f>0.12/1000</f>
-        <v>1.1999999999999999E-4</v>
+      <c r="H32" s="20">
+        <v>2.47E-2</v>
       </c>
       <c r="I32" s="21">
         <f t="shared" si="0"/>
@@ -3266,17 +3388,19 @@
       <c r="L32" s="7"/>
       <c r="M32" s="9"/>
     </row>
-    <row r="33" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D33" s="18"/>
+    <row r="33" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D33" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E33" s="18" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="F33" s="19"/>
       <c r="G33" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H33" s="20">
-        <v>8.9999999999999993E-3</v>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="I33" s="21">
         <f t="shared" si="0"/>
@@ -3287,17 +3411,19 @@
       <c r="L33" s="7"/>
       <c r="M33" s="9"/>
     </row>
-    <row r="34" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D34" s="18"/>
+    <row r="34" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D34" s="18" t="s">
+        <v>158</v>
+      </c>
       <c r="E34" s="18" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="F34" s="19"/>
       <c r="G34" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H34" s="20">
-        <v>3.8999999999999998E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="I34" s="21">
         <f t="shared" si="0"/>
@@ -3308,19 +3434,18 @@
       <c r="L34" s="7"/>
       <c r="M34" s="9"/>
     </row>
-    <row r="35" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D35" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E35" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="F35" s="19"/>
+    <row r="35" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D35" s="18"/>
+      <c r="E35" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="F35" s="28"/>
       <c r="G35" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="H35" s="20">
-        <v>2.1000000000000001E-2</v>
+      <c r="H35" s="29">
+        <f>0.12/1000</f>
+        <v>1.1999999999999999E-4</v>
       </c>
       <c r="I35" s="21">
         <f t="shared" si="0"/>
@@ -3331,17 +3456,17 @@
       <c r="L35" s="7"/>
       <c r="M35" s="9"/>
     </row>
-    <row r="36" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D36" s="18"/>
       <c r="E36" s="18" t="s">
-        <v>140</v>
+        <v>113</v>
       </c>
       <c r="F36" s="19"/>
       <c r="G36" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H36" s="20">
-        <v>2.5899999999999999E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="I36" s="21">
         <f t="shared" si="0"/>
@@ -3352,17 +3477,17 @@
       <c r="L36" s="7"/>
       <c r="M36" s="9"/>
     </row>
-    <row r="37" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D37" s="18"/>
       <c r="E37" s="18" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="F37" s="19"/>
       <c r="G37" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="H37" s="22">
-        <v>8.2500000000000004E-3</v>
+      <c r="H37" s="20">
+        <v>3.8999999999999998E-3</v>
       </c>
       <c r="I37" s="21">
         <f t="shared" si="0"/>
@@ -3373,19 +3498,19 @@
       <c r="L37" s="7"/>
       <c r="M37" s="9"/>
     </row>
-    <row r="38" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D38" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="F38" s="19"/>
       <c r="G38" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H38" s="20">
-        <v>4.2700000000000004E-3</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="I38" s="21">
         <f t="shared" si="0"/>
@@ -3396,17 +3521,17 @@
       <c r="L38" s="7"/>
       <c r="M38" s="9"/>
     </row>
-    <row r="39" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D39" s="18"/>
       <c r="E39" s="18" t="s">
-        <v>89</v>
+        <v>140</v>
       </c>
       <c r="F39" s="19"/>
       <c r="G39" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="H39" s="22">
-        <v>4.2700000000000004E-3</v>
+      <c r="H39" s="20">
+        <v>2.5899999999999999E-3</v>
       </c>
       <c r="I39" s="21">
         <f t="shared" si="0"/>
@@ -3417,19 +3542,17 @@
       <c r="L39" s="7"/>
       <c r="M39" s="9"/>
     </row>
-    <row r="40" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D40" s="18" t="s">
-        <v>21</v>
-      </c>
+    <row r="40" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D40" s="18"/>
       <c r="E40" s="18" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F40" s="19"/>
       <c r="G40" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="H40" s="20">
-        <v>4.79E-3</v>
+      <c r="H40" s="22">
+        <v>8.2500000000000004E-3</v>
       </c>
       <c r="I40" s="21">
         <f t="shared" si="0"/>
@@ -3440,38 +3563,42 @@
       <c r="L40" s="7"/>
       <c r="M40" s="9"/>
     </row>
-    <row r="41" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D41" s="18"/>
-      <c r="E41" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="F41" s="24"/>
-      <c r="G41" s="33" t="s">
+    <row r="41" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D41" s="46" t="s">
+        <v>201</v>
+      </c>
+      <c r="E41" s="45" t="s">
+        <v>202</v>
+      </c>
+      <c r="F41" s="45"/>
+      <c r="G41" s="20" t="s">
         <v>185</v>
       </c>
       <c r="H41" s="20">
-        <v>1.0000000000000001E-5</v>
+        <v>5.8E-4</v>
       </c>
       <c r="I41" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J41" s="8"/>
+      <c r="J41" s="7"/>
       <c r="K41" s="7"/>
       <c r="L41" s="7"/>
-      <c r="M41" s="10"/>
-    </row>
-    <row r="42" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D42" s="18"/>
+      <c r="M41" s="9"/>
+    </row>
+    <row r="42" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D42" s="18" t="s">
+        <v>20</v>
+      </c>
       <c r="E42" s="18" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F42" s="19"/>
       <c r="G42" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H42" s="20">
-        <v>7.5000000000000002E-4</v>
+        <v>4.2700000000000004E-3</v>
       </c>
       <c r="I42" s="21">
         <f t="shared" si="0"/>
@@ -3482,19 +3609,17 @@
       <c r="L42" s="7"/>
       <c r="M42" s="9"/>
     </row>
-    <row r="43" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D43" s="18" t="s">
-        <v>22</v>
-      </c>
+    <row r="43" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D43" s="18"/>
       <c r="E43" s="18" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="F43" s="19"/>
       <c r="G43" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="H43" s="20">
-        <v>3.5999999999999999E-3</v>
+      <c r="H43" s="22">
+        <v>4.2700000000000004E-3</v>
       </c>
       <c r="I43" s="21">
         <f t="shared" si="0"/>
@@ -3502,66 +3627,64 @@
       </c>
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
-      <c r="L43" s="8"/>
-      <c r="M43" s="10"/>
-    </row>
-    <row r="44" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D44" s="18"/>
-      <c r="E44" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="F44" s="24"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="9"/>
+    </row>
+    <row r="44" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D44" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="F44" s="19"/>
       <c r="G44" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H44" s="20">
-        <v>1.8610000000000002E-2</v>
+        <v>4.79E-3</v>
       </c>
       <c r="I44" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J44" s="8"/>
+      <c r="J44" s="7"/>
       <c r="K44" s="7"/>
       <c r="L44" s="7"/>
       <c r="M44" s="9"/>
     </row>
-    <row r="45" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D45" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E45" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="F45" s="19"/>
+    <row r="45" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D45" s="18"/>
+      <c r="E45" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="F45" s="24"/>
       <c r="G45" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H45" s="20">
-        <v>6.9999999999999994E-5</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="I45" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J45" s="7"/>
+      <c r="J45" s="8"/>
       <c r="K45" s="7"/>
       <c r="L45" s="7"/>
-      <c r="M45" s="9"/>
-    </row>
-    <row r="46" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D46" s="18" t="s">
-        <v>24</v>
-      </c>
+      <c r="M45" s="10"/>
+    </row>
+    <row r="46" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D46" s="18"/>
       <c r="E46" s="18" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F46" s="19"/>
       <c r="G46" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H46" s="20">
-        <v>4.0000000000000003E-5</v>
+        <v>7.5000000000000002E-4</v>
       </c>
       <c r="I46" s="21">
         <f t="shared" si="0"/>
@@ -3569,22 +3692,22 @@
       </c>
       <c r="J46" s="7"/>
       <c r="K46" s="7"/>
-      <c r="L46" s="8"/>
-      <c r="M46" s="10"/>
-    </row>
-    <row r="47" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="L46" s="7"/>
+      <c r="M46" s="9"/>
+    </row>
+    <row r="47" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D47" s="18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="F47" s="19"/>
       <c r="G47" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H47" s="20">
-        <v>1.0000000000000001E-5</v>
+        <v>3.5999999999999999E-3</v>
       </c>
       <c r="I47" s="21">
         <f t="shared" si="0"/>
@@ -3592,64 +3715,66 @@
       </c>
       <c r="J47" s="7"/>
       <c r="K47" s="7"/>
-      <c r="L47" s="7"/>
-      <c r="M47" s="9"/>
-    </row>
-    <row r="48" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D48" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E48" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="F48" s="19"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="10"/>
+    </row>
+    <row r="48" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D48" s="18"/>
+      <c r="E48" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="F48" s="24"/>
       <c r="G48" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H48" s="20">
-        <v>5.3E-3</v>
+        <v>1.8610000000000002E-2</v>
       </c>
       <c r="I48" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J48" s="7"/>
+      <c r="J48" s="8"/>
       <c r="K48" s="7"/>
       <c r="L48" s="7"/>
       <c r="M48" s="9"/>
     </row>
-    <row r="49" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D49" s="18"/>
+    <row r="49" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D49" s="18" t="s">
+        <v>23</v>
+      </c>
       <c r="E49" s="18" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="F49" s="19"/>
       <c r="G49" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H49" s="20">
-        <v>4.2799999999999998E-2</v>
+        <v>6.9999999999999994E-5</v>
       </c>
       <c r="I49" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J49" s="7"/>
-      <c r="K49" s="34"/>
+      <c r="K49" s="7"/>
       <c r="L49" s="7"/>
       <c r="M49" s="9"/>
     </row>
-    <row r="50" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D50" s="18"/>
+    <row r="50" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D50" s="18" t="s">
+        <v>24</v>
+      </c>
       <c r="E50" s="18" t="s">
-        <v>152</v>
+        <v>84</v>
       </c>
       <c r="F50" s="19"/>
       <c r="G50" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H50" s="20">
-        <v>7.9000000000000008E-3</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="I50" s="21">
         <f t="shared" si="0"/>
@@ -3657,22 +3782,22 @@
       </c>
       <c r="J50" s="7"/>
       <c r="K50" s="7"/>
-      <c r="L50" s="7"/>
-      <c r="M50" s="9"/>
-    </row>
-    <row r="51" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="L50" s="8"/>
+      <c r="M50" s="10"/>
+    </row>
+    <row r="51" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D51" s="18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F51" s="19"/>
       <c r="G51" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H51" s="20">
-        <v>7.2399999999999999E-3</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="I51" s="21">
         <f t="shared" si="0"/>
@@ -3683,17 +3808,19 @@
       <c r="L51" s="7"/>
       <c r="M51" s="9"/>
     </row>
-    <row r="52" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D52" s="18"/>
+    <row r="52" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D52" s="18" t="s">
+        <v>26</v>
+      </c>
       <c r="E52" s="18" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="F52" s="19"/>
       <c r="G52" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H52" s="20">
-        <v>2.2000000000000001E-3</v>
+        <v>5.3E-3</v>
       </c>
       <c r="I52" s="21">
         <f t="shared" si="0"/>
@@ -3704,40 +3831,38 @@
       <c r="L52" s="7"/>
       <c r="M52" s="9"/>
     </row>
-    <row r="53" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D53" s="18"/>
       <c r="E53" s="18" t="s">
-        <v>81</v>
+        <v>116</v>
       </c>
       <c r="F53" s="19"/>
       <c r="G53" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H53" s="20">
-        <v>1.0000000000000001E-5</v>
+        <v>4.2799999999999998E-2</v>
       </c>
       <c r="I53" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J53" s="7"/>
-      <c r="K53" s="7"/>
+      <c r="K53" s="34"/>
       <c r="L53" s="7"/>
       <c r="M53" s="9"/>
     </row>
-    <row r="54" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D54" s="18" t="s">
-        <v>28</v>
-      </c>
+    <row r="54" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D54" s="18"/>
       <c r="E54" s="18" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="F54" s="19"/>
       <c r="G54" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H54" s="20">
-        <v>1.12E-2</v>
+        <v>7.9000000000000008E-3</v>
       </c>
       <c r="I54" s="21">
         <f t="shared" si="0"/>
@@ -3748,59 +3873,61 @@
       <c r="L54" s="7"/>
       <c r="M54" s="9"/>
     </row>
-    <row r="55" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D55" s="18"/>
-      <c r="E55" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="F55" s="24"/>
+    <row r="55" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D55" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E55" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F55" s="19"/>
       <c r="G55" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H55" s="20">
-        <v>2.9E-4</v>
+        <v>7.2399999999999999E-3</v>
       </c>
       <c r="I55" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J55" s="8"/>
+      <c r="J55" s="7"/>
       <c r="K55" s="7"/>
       <c r="L55" s="7"/>
       <c r="M55" s="9"/>
     </row>
-    <row r="56" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D56" s="18"/>
       <c r="E56" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="F56" s="24"/>
+        <v>143</v>
+      </c>
+      <c r="F56" s="19"/>
       <c r="G56" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H56" s="20">
-        <v>0.1074</v>
+        <v>2.2000000000000001E-3</v>
       </c>
       <c r="I56" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J56" s="8"/>
+      <c r="J56" s="7"/>
       <c r="K56" s="7"/>
       <c r="L56" s="7"/>
       <c r="M56" s="9"/>
     </row>
-    <row r="57" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D57" s="18"/>
       <c r="E57" s="18" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="F57" s="19"/>
       <c r="G57" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H57" s="20">
-        <v>1.64E-3</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="I57" s="21">
         <f t="shared" si="0"/>
@@ -3808,22 +3935,22 @@
       </c>
       <c r="J57" s="7"/>
       <c r="K57" s="7"/>
-      <c r="L57" s="8"/>
-      <c r="M57" s="10"/>
-    </row>
-    <row r="58" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="L57" s="7"/>
+      <c r="M57" s="9"/>
+    </row>
+    <row r="58" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D58" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E58" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F58" s="19"/>
       <c r="G58" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H58" s="20">
-        <v>1.43E-2</v>
+        <v>1.12E-2</v>
       </c>
       <c r="I58" s="21">
         <f t="shared" si="0"/>
@@ -3834,63 +3961,59 @@
       <c r="L58" s="7"/>
       <c r="M58" s="9"/>
     </row>
-    <row r="59" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D59" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E59" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="F59" s="19"/>
+    <row r="59" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D59" s="18"/>
+      <c r="E59" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="F59" s="24"/>
       <c r="G59" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H59" s="20">
-        <v>3.7000000000000002E-3</v>
+        <v>2.9E-4</v>
       </c>
       <c r="I59" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J59" s="7"/>
+      <c r="J59" s="8"/>
       <c r="K59" s="7"/>
       <c r="L59" s="7"/>
       <c r="M59" s="9"/>
     </row>
-    <row r="60" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D60" s="18"/>
       <c r="E60" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="F60" s="19"/>
+        <v>117</v>
+      </c>
+      <c r="F60" s="24"/>
       <c r="G60" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H60" s="20">
-        <v>8.2500000000000004E-3</v>
+        <v>0.1074</v>
       </c>
       <c r="I60" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J60" s="7"/>
+      <c r="J60" s="8"/>
       <c r="K60" s="7"/>
       <c r="L60" s="7"/>
       <c r="M60" s="9"/>
     </row>
-    <row r="61" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D61" s="18" t="s">
-        <v>159</v>
-      </c>
+    <row r="61" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D61" s="18"/>
       <c r="E61" s="18" t="s">
-        <v>121</v>
+        <v>53</v>
       </c>
       <c r="F61" s="19"/>
       <c r="G61" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H61" s="20">
-        <v>1.7299999999999999E-2</v>
+        <v>1.64E-3</v>
       </c>
       <c r="I61" s="21">
         <f t="shared" si="0"/>
@@ -3898,43 +4021,45 @@
       </c>
       <c r="J61" s="7"/>
       <c r="K61" s="7"/>
-      <c r="L61" s="7"/>
-      <c r="M61" s="9"/>
-    </row>
-    <row r="62" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D62" s="18"/>
-      <c r="E62" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="F62" s="24"/>
-      <c r="G62" s="33" t="s">
+      <c r="L61" s="8"/>
+      <c r="M61" s="10"/>
+    </row>
+    <row r="62" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D62" s="46" t="s">
+        <v>203</v>
+      </c>
+      <c r="E62" s="47" t="s">
+        <v>203</v>
+      </c>
+      <c r="F62" s="45"/>
+      <c r="G62" s="20" t="s">
         <v>185</v>
       </c>
       <c r="H62" s="20">
-        <v>1.0000000000000001E-5</v>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="I62" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J62" s="8"/>
+      <c r="J62" s="7"/>
       <c r="K62" s="7"/>
-      <c r="L62" s="7"/>
-      <c r="M62" s="9"/>
-    </row>
-    <row r="63" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="L62" s="8"/>
+      <c r="M62" s="10"/>
+    </row>
+    <row r="63" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D63" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E63" s="18" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="F63" s="19"/>
       <c r="G63" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H63" s="20">
-        <v>7.3000000000000001E-3</v>
+        <v>1.43E-2</v>
       </c>
       <c r="I63" s="21">
         <f t="shared" si="0"/>
@@ -3945,19 +4070,19 @@
       <c r="L63" s="7"/>
       <c r="M63" s="9"/>
     </row>
-    <row r="64" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D64" s="18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E64" s="18" t="s">
-        <v>77</v>
+        <v>120</v>
       </c>
       <c r="F64" s="19"/>
       <c r="G64" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H64" s="20">
-        <v>3.49E-3</v>
+        <v>3.7000000000000002E-3</v>
       </c>
       <c r="I64" s="21">
         <f t="shared" si="0"/>
@@ -3965,22 +4090,20 @@
       </c>
       <c r="J64" s="7"/>
       <c r="K64" s="7"/>
-      <c r="L64" s="8"/>
-      <c r="M64" s="10"/>
-    </row>
-    <row r="65" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D65" s="18" t="s">
-        <v>33</v>
-      </c>
+      <c r="L64" s="7"/>
+      <c r="M64" s="9"/>
+    </row>
+    <row r="65" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D65" s="18"/>
       <c r="E65" s="18" t="s">
-        <v>122</v>
+        <v>79</v>
       </c>
       <c r="F65" s="19"/>
       <c r="G65" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H65" s="20">
-        <v>4.07E-2</v>
+        <v>8.2500000000000004E-3</v>
       </c>
       <c r="I65" s="21">
         <f t="shared" si="0"/>
@@ -3991,19 +4114,19 @@
       <c r="L65" s="7"/>
       <c r="M65" s="9"/>
     </row>
-    <row r="66" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D66" s="18" t="s">
-        <v>34</v>
+        <v>159</v>
       </c>
       <c r="E66" s="18" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F66" s="19"/>
       <c r="G66" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H66" s="20">
-        <v>6.3E-3</v>
+        <v>1.7299999999999999E-2</v>
       </c>
       <c r="I66" s="21">
         <f t="shared" si="0"/>
@@ -4014,42 +4137,40 @@
       <c r="L66" s="7"/>
       <c r="M66" s="9"/>
     </row>
-    <row r="67" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D67" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E67" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="F67" s="19"/>
+    <row r="67" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D67" s="18"/>
+      <c r="E67" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="F67" s="24"/>
       <c r="G67" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H67" s="20">
-        <v>1.0999999999999999E-2</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="I67" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J67" s="7"/>
+      <c r="J67" s="8"/>
       <c r="K67" s="7"/>
       <c r="L67" s="7"/>
       <c r="M67" s="9"/>
     </row>
-    <row r="68" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D68" s="18" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="E68" s="18" t="s">
-        <v>55</v>
+        <v>144</v>
       </c>
       <c r="F68" s="19"/>
       <c r="G68" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H68" s="20">
-        <v>6.0000000000000002E-5</v>
+        <v>7.3000000000000001E-3</v>
       </c>
       <c r="I68" s="21">
         <f t="shared" si="0"/>
@@ -4060,17 +4181,19 @@
       <c r="L68" s="7"/>
       <c r="M68" s="9"/>
     </row>
-    <row r="69" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D69" s="18"/>
-      <c r="E69" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="F69" s="19"/>
-      <c r="G69" s="33" t="s">
+    <row r="69" spans="4:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D69" s="46" t="s">
+        <v>204</v>
+      </c>
+      <c r="E69" s="47" t="s">
+        <v>205</v>
+      </c>
+      <c r="F69" s="45"/>
+      <c r="G69" s="20" t="s">
         <v>185</v>
       </c>
       <c r="H69" s="20">
-        <v>1.0000000000000001E-5</v>
+        <v>9.2549999999999993E-2</v>
       </c>
       <c r="I69" s="21">
         <f t="shared" si="0"/>
@@ -4081,19 +4204,19 @@
       <c r="L69" s="7"/>
       <c r="M69" s="9"/>
     </row>
-    <row r="70" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D70" s="18" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E70" s="18" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F70" s="19"/>
       <c r="G70" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H70" s="20">
-        <v>1.0000000000000001E-5</v>
+        <v>3.49E-3</v>
       </c>
       <c r="I70" s="21">
         <f t="shared" si="0"/>
@@ -4101,69 +4224,71 @@
       </c>
       <c r="J70" s="7"/>
       <c r="K70" s="7"/>
-      <c r="L70" s="7"/>
-      <c r="M70" s="9"/>
-    </row>
-    <row r="71" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D71" s="18"/>
-      <c r="E71" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="F71" s="24"/>
+      <c r="L70" s="8"/>
+      <c r="M70" s="10"/>
+    </row>
+    <row r="71" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D71" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E71" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="F71" s="19"/>
       <c r="G71" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H71" s="20">
-        <v>1.0000000000000001E-5</v>
+        <v>4.07E-2</v>
       </c>
       <c r="I71" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J71" s="8"/>
+      <c r="J71" s="7"/>
       <c r="K71" s="7"/>
       <c r="L71" s="7"/>
       <c r="M71" s="9"/>
     </row>
-    <row r="72" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D72" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="E72" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="F72" s="24"/>
+        <v>34</v>
+      </c>
+      <c r="E72" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="F72" s="19"/>
       <c r="G72" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H72" s="20">
-        <v>1.3999999999999999E-4</v>
+        <v>6.3E-3</v>
       </c>
       <c r="I72" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J72" s="8"/>
+      <c r="J72" s="7"/>
       <c r="K72" s="7"/>
       <c r="L72" s="7"/>
       <c r="M72" s="9"/>
     </row>
-    <row r="73" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D73" s="18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E73" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F73" s="19"/>
       <c r="G73" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H73" s="20">
-        <v>2.9000000000000001E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="I73" s="21">
-        <f t="shared" ref="I73:I102" si="1">IF(G73&lt;&gt;"-",G73*H73,F73*H73)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J73" s="7"/>
@@ -4171,12 +4296,12 @@
       <c r="L73" s="7"/>
       <c r="M73" s="9"/>
     </row>
-    <row r="74" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D74" s="18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E74" s="18" t="s">
-        <v>146</v>
+        <v>55</v>
       </c>
       <c r="F74" s="19"/>
       <c r="G74" s="33" t="s">
@@ -4186,7 +4311,7 @@
         <v>6.0000000000000002E-5</v>
       </c>
       <c r="I74" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J74" s="7"/>
@@ -4194,20 +4319,20 @@
       <c r="L74" s="7"/>
       <c r="M74" s="9"/>
     </row>
-    <row r="75" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D75" s="18"/>
       <c r="E75" s="18" t="s">
-        <v>147</v>
+        <v>74</v>
       </c>
       <c r="F75" s="19"/>
       <c r="G75" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="H75" s="22">
-        <v>6.9999999999999994E-5</v>
+      <c r="H75" s="20">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="I75" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J75" s="7"/>
@@ -4215,87 +4340,89 @@
       <c r="L75" s="7"/>
       <c r="M75" s="9"/>
     </row>
-    <row r="76" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D76" s="18"/>
+    <row r="76" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D76" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="E76" s="18" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F76" s="19"/>
       <c r="G76" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="H76" s="22">
-        <v>9.0000000000000006E-5</v>
+      <c r="H76" s="20">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="I76" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J76" s="7"/>
       <c r="K76" s="7"/>
-      <c r="L76" s="8"/>
-      <c r="M76" s="10"/>
-    </row>
-    <row r="77" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="L76" s="7"/>
+      <c r="M76" s="9"/>
+    </row>
+    <row r="77" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D77" s="18"/>
-      <c r="E77" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="F77" s="19"/>
+      <c r="E77" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="F77" s="24"/>
       <c r="G77" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="H77" s="22">
-        <v>6.9999999999999994E-5</v>
+      <c r="H77" s="20">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="I77" s="21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J77" s="7"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J77" s="8"/>
       <c r="K77" s="7"/>
-      <c r="L77" s="8"/>
-      <c r="M77" s="10"/>
-    </row>
-    <row r="78" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="L77" s="7"/>
+      <c r="M77" s="9"/>
+    </row>
+    <row r="78" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D78" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E78" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="F78" s="19"/>
+        <v>57</v>
+      </c>
+      <c r="E78" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="F78" s="24"/>
       <c r="G78" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H78" s="20">
-        <v>5.7200000000000003E-3</v>
+        <v>1.3999999999999999E-4</v>
       </c>
       <c r="I78" s="21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J78" s="7"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J78" s="8"/>
       <c r="K78" s="7"/>
       <c r="L78" s="7"/>
       <c r="M78" s="9"/>
     </row>
-    <row r="79" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D79" s="18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E79" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F79" s="19"/>
       <c r="G79" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H79" s="20">
-        <v>4.36E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="I79" s="21">
-        <f>IF(G79&lt;&gt;"-",G79*H79,F79*H79)</f>
+        <f t="shared" ref="I79:I110" si="1">IF(G79&lt;&gt;"-",G79*H79,F79*H79)</f>
         <v>0</v>
       </c>
       <c r="J79" s="7"/>
@@ -4303,19 +4430,19 @@
       <c r="L79" s="7"/>
       <c r="M79" s="9"/>
     </row>
-    <row r="80" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D80" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="E80" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="F80" s="19"/>
-      <c r="G80" s="33" t="s">
+    <row r="80" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D80" s="44" t="s">
+        <v>206</v>
+      </c>
+      <c r="E80" s="45" t="s">
+        <v>207</v>
+      </c>
+      <c r="F80" s="45"/>
+      <c r="G80" s="20" t="s">
         <v>185</v>
       </c>
       <c r="H80" s="20">
-        <v>1.3100000000000001E-2</v>
+        <v>1.47E-3</v>
       </c>
       <c r="I80" s="21">
         <f t="shared" si="1"/>
@@ -4324,20 +4451,21 @@
       <c r="J80" s="7"/>
       <c r="K80" s="7"/>
       <c r="L80" s="7"/>
-      <c r="M80" s="10"/>
-    </row>
-    <row r="81" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D81" s="18"/>
-      <c r="E81" s="27" t="s">
-        <v>155</v>
-      </c>
-      <c r="F81" s="28"/>
+      <c r="M80" s="9"/>
+    </row>
+    <row r="81" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D81" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E81" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F81" s="19"/>
       <c r="G81" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="H81" s="29">
-        <f>24.2/1000</f>
-        <v>2.4199999999999999E-2</v>
+      <c r="H81" s="20">
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="I81" s="21">
         <f t="shared" si="1"/>
@@ -4346,21 +4474,19 @@
       <c r="J81" s="7"/>
       <c r="K81" s="7"/>
       <c r="L81" s="7"/>
-      <c r="M81" s="10"/>
-    </row>
-    <row r="82" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D82" s="18" t="s">
-        <v>41</v>
-      </c>
+      <c r="M81" s="9"/>
+    </row>
+    <row r="82" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D82" s="18"/>
       <c r="E82" s="18" t="s">
-        <v>128</v>
+        <v>147</v>
       </c>
       <c r="F82" s="19"/>
       <c r="G82" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="H82" s="20">
-        <v>1.9900000000000001E-2</v>
+      <c r="H82" s="22">
+        <v>6.9999999999999994E-5</v>
       </c>
       <c r="I82" s="21">
         <f t="shared" si="1"/>
@@ -4369,19 +4495,19 @@
       <c r="J82" s="7"/>
       <c r="K82" s="7"/>
       <c r="L82" s="7"/>
-      <c r="M82" s="10"/>
-    </row>
-    <row r="83" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M82" s="9"/>
+    </row>
+    <row r="83" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D83" s="18"/>
       <c r="E83" s="18" t="s">
-        <v>129</v>
+        <v>72</v>
       </c>
       <c r="F83" s="19"/>
       <c r="G83" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="H83" s="20">
-        <v>7.4000000000000003E-3</v>
+      <c r="H83" s="22">
+        <v>9.0000000000000006E-5</v>
       </c>
       <c r="I83" s="21">
         <f t="shared" si="1"/>
@@ -4389,22 +4515,20 @@
       </c>
       <c r="J83" s="7"/>
       <c r="K83" s="7"/>
-      <c r="L83" s="7"/>
+      <c r="L83" s="8"/>
       <c r="M83" s="10"/>
     </row>
-    <row r="84" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D84" s="18" t="s">
-        <v>42</v>
-      </c>
+    <row r="84" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D84" s="18"/>
       <c r="E84" s="18" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F84" s="19"/>
       <c r="G84" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="H84" s="20">
-        <v>5.5000000000000003E-4</v>
+      <c r="H84" s="22">
+        <v>6.9999999999999994E-5</v>
       </c>
       <c r="I84" s="21">
         <f t="shared" si="1"/>
@@ -4412,22 +4536,20 @@
       </c>
       <c r="J84" s="7"/>
       <c r="K84" s="7"/>
-      <c r="L84" s="7"/>
-      <c r="M84" s="9"/>
-    </row>
-    <row r="85" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D85" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E85" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="F85" s="19"/>
-      <c r="G85" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="H85" s="22">
-        <v>2.5899999999999999E-3</v>
+      <c r="L84" s="8"/>
+      <c r="M84" s="10"/>
+    </row>
+    <row r="85" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D85" s="46"/>
+      <c r="E85" s="45" t="s">
+        <v>208</v>
+      </c>
+      <c r="F85" s="45"/>
+      <c r="G85" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="H85" s="20">
+        <v>3.1800000000000002E-2</v>
       </c>
       <c r="I85" s="21">
         <f t="shared" si="1"/>
@@ -4435,22 +4557,22 @@
       </c>
       <c r="J85" s="7"/>
       <c r="K85" s="7"/>
-      <c r="L85" s="7"/>
-      <c r="M85" s="9"/>
-    </row>
-    <row r="86" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="L85" s="8"/>
+      <c r="M85" s="10"/>
+    </row>
+    <row r="86" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D86" s="18" t="s">
-        <v>160</v>
+        <v>38</v>
       </c>
       <c r="E86" s="18" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="F86" s="19"/>
       <c r="G86" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="H86" s="22">
-        <v>1.18E-2</v>
+      <c r="H86" s="20">
+        <v>5.7200000000000003E-3</v>
       </c>
       <c r="I86" s="21">
         <f t="shared" si="1"/>
@@ -4461,22 +4583,22 @@
       <c r="L86" s="7"/>
       <c r="M86" s="9"/>
     </row>
-    <row r="87" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D87" s="18" t="s">
-        <v>161</v>
+        <v>39</v>
       </c>
       <c r="E87" s="18" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F87" s="19"/>
       <c r="G87" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="H87" s="22">
-        <v>2.3199999999999998E-2</v>
+      <c r="H87" s="20">
+        <v>4.36E-2</v>
       </c>
       <c r="I87" s="21">
-        <f t="shared" si="1"/>
+        <f>IF(G87&lt;&gt;"-",G87*H87,F87*H87)</f>
         <v>0</v>
       </c>
       <c r="J87" s="7"/>
@@ -4484,17 +4606,19 @@
       <c r="L87" s="7"/>
       <c r="M87" s="9"/>
     </row>
-    <row r="88" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D88" s="18"/>
+    <row r="88" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D88" s="18" t="s">
+        <v>40</v>
+      </c>
       <c r="E88" s="18" t="s">
-        <v>67</v>
+        <v>127</v>
       </c>
       <c r="F88" s="19"/>
       <c r="G88" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H88" s="20">
-        <v>1.01E-3</v>
+        <v>1.3100000000000001E-2</v>
       </c>
       <c r="I88" s="21">
         <f t="shared" si="1"/>
@@ -4503,19 +4627,20 @@
       <c r="J88" s="7"/>
       <c r="K88" s="7"/>
       <c r="L88" s="7"/>
-      <c r="M88" s="9"/>
-    </row>
-    <row r="89" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M88" s="10"/>
+    </row>
+    <row r="89" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D89" s="18"/>
-      <c r="E89" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="F89" s="19"/>
+      <c r="E89" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="F89" s="28"/>
       <c r="G89" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="H89" s="22">
-        <v>1.0000000000000001E-5</v>
+      <c r="H89" s="29">
+        <f>24.2/1000</f>
+        <v>2.4199999999999999E-2</v>
       </c>
       <c r="I89" s="21">
         <f t="shared" si="1"/>
@@ -4524,19 +4649,21 @@
       <c r="J89" s="7"/>
       <c r="K89" s="7"/>
       <c r="L89" s="7"/>
-      <c r="M89" s="9"/>
-    </row>
-    <row r="90" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D90" s="18"/>
+      <c r="M89" s="10"/>
+    </row>
+    <row r="90" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D90" s="18" t="s">
+        <v>41</v>
+      </c>
       <c r="E90" s="18" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="F90" s="19"/>
       <c r="G90" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H90" s="20">
-        <v>5.8799999999999998E-3</v>
+        <v>1.9900000000000001E-2</v>
       </c>
       <c r="I90" s="21">
         <f t="shared" si="1"/>
@@ -4547,19 +4674,17 @@
       <c r="L90" s="7"/>
       <c r="M90" s="10"/>
     </row>
-    <row r="91" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D91" s="18" t="s">
-        <v>44</v>
-      </c>
+    <row r="91" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D91" s="18"/>
       <c r="E91" s="18" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="F91" s="19"/>
       <c r="G91" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H91" s="20">
-        <v>4.2700000000000004E-3</v>
+        <v>7.4000000000000003E-3</v>
       </c>
       <c r="I91" s="21">
         <f t="shared" si="1"/>
@@ -4570,19 +4695,19 @@
       <c r="L91" s="7"/>
       <c r="M91" s="10"/>
     </row>
-    <row r="92" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="92" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D92" s="18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E92" s="18" t="s">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="F92" s="19"/>
       <c r="G92" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H92" s="20">
-        <v>5.4000000000000003E-3</v>
+        <v>5.5000000000000003E-4</v>
       </c>
       <c r="I92" s="21">
         <f t="shared" si="1"/>
@@ -4591,21 +4716,21 @@
       <c r="J92" s="7"/>
       <c r="K92" s="7"/>
       <c r="L92" s="7"/>
-      <c r="M92" s="10"/>
-    </row>
-    <row r="93" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M92" s="9"/>
+    </row>
+    <row r="93" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D93" s="18" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="E93" s="18" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F93" s="19"/>
       <c r="G93" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="H93" s="20">
-        <v>1.0970000000000001E-2</v>
+      <c r="H93" s="22">
+        <v>2.5899999999999999E-3</v>
       </c>
       <c r="I93" s="21">
         <f t="shared" si="1"/>
@@ -4616,19 +4741,19 @@
       <c r="L93" s="7"/>
       <c r="M93" s="9"/>
     </row>
-    <row r="94" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D94" s="18" t="s">
-        <v>46</v>
+        <v>160</v>
       </c>
       <c r="E94" s="18" t="s">
-        <v>65</v>
+        <v>153</v>
       </c>
       <c r="F94" s="19"/>
       <c r="G94" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H94" s="22">
-        <v>1.65E-3</v>
+        <v>1.18E-2</v>
       </c>
       <c r="I94" s="21">
         <f t="shared" si="1"/>
@@ -4637,19 +4762,21 @@
       <c r="J94" s="7"/>
       <c r="K94" s="7"/>
       <c r="L94" s="7"/>
-      <c r="M94" s="10"/>
-    </row>
-    <row r="95" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D95" s="18"/>
+      <c r="M94" s="9"/>
+    </row>
+    <row r="95" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D95" s="18" t="s">
+        <v>161</v>
+      </c>
       <c r="E95" s="18" t="s">
-        <v>64</v>
+        <v>130</v>
       </c>
       <c r="F95" s="19"/>
       <c r="G95" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="H95" s="20">
-        <v>3.49E-3</v>
+      <c r="H95" s="22">
+        <v>2.3199999999999998E-2</v>
       </c>
       <c r="I95" s="21">
         <f t="shared" si="1"/>
@@ -4660,18 +4787,17 @@
       <c r="L95" s="7"/>
       <c r="M95" s="9"/>
     </row>
-    <row r="96" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D96" s="18"/>
-      <c r="E96" s="27" t="s">
-        <v>154</v>
-      </c>
-      <c r="F96" s="28"/>
+      <c r="E96" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="F96" s="19"/>
       <c r="G96" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="H96" s="29">
-        <f>7.59/1000</f>
-        <v>7.5899999999999995E-3</v>
+      <c r="H96" s="20">
+        <v>1.01E-3</v>
       </c>
       <c r="I96" s="21">
         <f t="shared" si="1"/>
@@ -4682,17 +4808,17 @@
       <c r="L96" s="7"/>
       <c r="M96" s="9"/>
     </row>
-    <row r="97" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D97" s="18"/>
       <c r="E97" s="18" t="s">
-        <v>131</v>
+        <v>68</v>
       </c>
       <c r="F97" s="19"/>
       <c r="G97" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H97" s="22">
-        <v>4.2000000000000003E-2</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="I97" s="21">
         <f t="shared" si="1"/>
@@ -4703,40 +4829,40 @@
       <c r="L97" s="7"/>
       <c r="M97" s="9"/>
     </row>
-    <row r="98" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="98" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D98" s="18"/>
       <c r="E98" s="18" t="s">
-        <v>63</v>
+        <v>149</v>
       </c>
       <c r="F98" s="19"/>
       <c r="G98" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H98" s="20">
-        <v>1.01E-3</v>
+        <v>5.8799999999999998E-3</v>
       </c>
       <c r="I98" s="21">
-        <f>IF(G98&lt;&gt;"-",G98*H98,F98*H98)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J98" s="7"/>
       <c r="K98" s="7"/>
       <c r="L98" s="7"/>
-      <c r="M98" s="9"/>
-    </row>
-    <row r="99" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M98" s="10"/>
+    </row>
+    <row r="99" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D99" s="18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E99" s="18" t="s">
-        <v>62</v>
+        <v>148</v>
       </c>
       <c r="F99" s="19"/>
       <c r="G99" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H99" s="20">
-        <v>5.5999999999999995E-4</v>
+        <v>4.2700000000000004E-3</v>
       </c>
       <c r="I99" s="21">
         <f t="shared" si="1"/>
@@ -4745,21 +4871,21 @@
       <c r="J99" s="7"/>
       <c r="K99" s="7"/>
       <c r="L99" s="7"/>
-      <c r="M99" s="9"/>
-    </row>
-    <row r="100" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M99" s="10"/>
+    </row>
+    <row r="100" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D100" s="18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E100" s="18" t="s">
-        <v>61</v>
+        <v>105</v>
       </c>
       <c r="F100" s="19"/>
       <c r="G100" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H100" s="20">
-        <v>3.9E-2</v>
+        <v>5.4000000000000003E-3</v>
       </c>
       <c r="I100" s="21">
         <f t="shared" si="1"/>
@@ -4770,19 +4896,19 @@
       <c r="L100" s="7"/>
       <c r="M100" s="10"/>
     </row>
-    <row r="101" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D101" s="18" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E101" s="18" t="s">
-        <v>132</v>
+        <v>66</v>
       </c>
       <c r="F101" s="19"/>
       <c r="G101" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H101" s="20">
-        <v>4.7999999999999996E-3</v>
+        <v>1.0970000000000001E-2</v>
       </c>
       <c r="I101" s="21">
         <f t="shared" si="1"/>
@@ -4793,69 +4919,246 @@
       <c r="L101" s="7"/>
       <c r="M101" s="9"/>
     </row>
-    <row r="102" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="102" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D102" s="18" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E102" s="18" t="s">
-        <v>133</v>
+        <v>65</v>
       </c>
       <c r="F102" s="19"/>
       <c r="G102" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="H102" s="20">
-        <v>2.4E-2</v>
+      <c r="H102" s="22">
+        <v>1.65E-3</v>
       </c>
       <c r="I102" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="J102" s="7"/>
+      <c r="K102" s="7"/>
       <c r="L102" s="7"/>
       <c r="M102" s="10"/>
     </row>
-    <row r="103" spans="4:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="103" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D103" s="18"/>
       <c r="E103" s="18" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F103" s="19"/>
       <c r="G103" s="33" t="s">
         <v>185</v>
       </c>
       <c r="H103" s="20">
-        <v>1.0000000000000001E-5</v>
+        <v>3.49E-3</v>
       </c>
       <c r="I103" s="21">
-        <f>IF(G103&lt;&gt;"-",G103*H103,F103*H103)</f>
-        <v>0</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J103" s="7"/>
+      <c r="K103" s="7"/>
       <c r="L103" s="7"/>
       <c r="M103" s="9"/>
     </row>
-    <row r="104" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D104" s="18"/>
+      <c r="E104" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="F104" s="28"/>
+      <c r="G104" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="H104" s="29">
+        <f>7.59/1000</f>
+        <v>7.5899999999999995E-3</v>
+      </c>
+      <c r="I104" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J104" s="7"/>
+      <c r="K104" s="7"/>
       <c r="L104" s="7"/>
       <c r="M104" s="9"/>
     </row>
-    <row r="105" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D105" s="18"/>
+      <c r="E105" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="F105" s="19"/>
+      <c r="G105" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="H105" s="22">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="I105" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J105" s="7"/>
+      <c r="K105" s="7"/>
       <c r="L105" s="7"/>
-      <c r="M105" s="10"/>
-    </row>
-    <row r="106" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M105" s="9"/>
+    </row>
+    <row r="106" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D106" s="18"/>
+      <c r="E106" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F106" s="19"/>
+      <c r="G106" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="H106" s="20">
+        <v>1.01E-3</v>
+      </c>
+      <c r="I106" s="21">
+        <f>IF(G106&lt;&gt;"-",G106*H106,F106*H106)</f>
+        <v>0</v>
+      </c>
+      <c r="J106" s="7"/>
+      <c r="K106" s="7"/>
       <c r="L106" s="7"/>
       <c r="M106" s="9"/>
     </row>
-    <row r="107" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D107" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E107" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F107" s="19"/>
+      <c r="G107" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="H107" s="20">
+        <v>5.5999999999999995E-4</v>
+      </c>
+      <c r="I107" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J107" s="7"/>
+      <c r="K107" s="7"/>
       <c r="L107" s="7"/>
       <c r="M107" s="9"/>
     </row>
-    <row r="108" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D108" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E108" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F108" s="19"/>
+      <c r="G108" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="H108" s="20">
+        <v>3.9E-2</v>
+      </c>
+      <c r="I108" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J108" s="7"/>
+      <c r="K108" s="7"/>
       <c r="L108" s="7"/>
-      <c r="M108" s="9"/>
+      <c r="M108" s="10"/>
+    </row>
+    <row r="109" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D109" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E109" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="F109" s="19"/>
+      <c r="G109" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="H109" s="20">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="I109" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J109" s="7"/>
+      <c r="K109" s="7"/>
+      <c r="L109" s="7"/>
+      <c r="M109" s="9"/>
+    </row>
+    <row r="110" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D110" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E110" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="F110" s="19"/>
+      <c r="G110" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="H110" s="20">
+        <v>2.4E-2</v>
+      </c>
+      <c r="I110" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L110" s="7"/>
+      <c r="M110" s="10"/>
+    </row>
+    <row r="111" spans="4:13" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="D111" s="18"/>
+      <c r="E111" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F111" s="19"/>
+      <c r="G111" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="H111" s="20">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I111" s="21">
+        <f>IF(G111&lt;&gt;"-",G111*H111,F111*H111)</f>
+        <v>0</v>
+      </c>
+      <c r="L111" s="7"/>
+      <c r="M111" s="9"/>
+    </row>
+    <row r="112" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="L112" s="7"/>
+      <c r="M112" s="9"/>
+    </row>
+    <row r="113" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L113" s="7"/>
+      <c r="M113" s="10"/>
+    </row>
+    <row r="114" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L114" s="7"/>
+      <c r="M114" s="9"/>
+    </row>
+    <row r="115" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L115" s="7"/>
+      <c r="M115" s="9"/>
+    </row>
+    <row r="116" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L116" s="7"/>
+      <c r="M116" s="9"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" autoFilter="0"/>
-  <autoFilter ref="D7:I103" xr:uid="{CE9FD823-0127-4C95-94F5-6E3964FBBD64}"/>
+  <autoFilter ref="D7:I111" xr:uid="{CE9FD823-0127-4C95-94F5-6E3964FBBD64}"/>
   <mergeCells count="3">
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="E1:G1"/>
@@ -4874,14 +5177,14 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.33203125" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="31" t="s">
         <v>162</v>
       </c>
@@ -4892,7 +5195,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>165</v>
       </c>
@@ -4903,7 +5206,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>167</v>
       </c>
@@ -4914,7 +5217,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>171</v>
       </c>
@@ -4925,7 +5228,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>175</v>
       </c>
@@ -4936,7 +5239,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>177</v>
       </c>
@@ -4947,7 +5250,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>181</v>
       </c>
@@ -4958,17 +5261,17 @@
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>187</v>
       </c>
@@ -4979,7 +5282,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>190</v>
       </c>
@@ -4994,26 +5297,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fc7f534a-70fb-4324-b2e1-98e1059d7272">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="711517d2-f3f9-44d8-b49d-51b2d5d7a8cc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010077DC2D14F6B96844AFA931507725A7DF" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0958de7b4e2e166f8e15808be88d1eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fc7f534a-70fb-4324-b2e1-98e1059d7272" xmlns:ns3="711517d2-f3f9-44d8-b49d-51b2d5d7a8cc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8cbc3ffa19650d64a3bc623f926a7ea7" ns2:_="" ns3:_="">
     <xsd:import namespace="fc7f534a-70fb-4324-b2e1-98e1059d7272"/>
@@ -5220,32 +5503,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC6A370F-DF6F-44BA-B49A-841CC5CF9C2D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="711517d2-f3f9-44d8-b49d-51b2d5d7a8cc"/>
-    <ds:schemaRef ds:uri="fc7f534a-70fb-4324-b2e1-98e1059d7272"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{964F8CBE-4092-4914-91BB-53FDFA321D0D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fc7f534a-70fb-4324-b2e1-98e1059d7272">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="711517d2-f3f9-44d8-b49d-51b2d5d7a8cc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89FFA54B-5E98-48BF-B353-DD83C478B505}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5264,6 +5542,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{964F8CBE-4092-4914-91BB-53FDFA321D0D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC6A370F-DF6F-44BA-B49A-841CC5CF9C2D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="711517d2-f3f9-44d8-b49d-51b2d5d7a8cc"/>
+    <ds:schemaRef ds:uri="fc7f534a-70fb-4324-b2e1-98e1059d7272"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{ed006307-e4a9-430f-af16-eea280431306}" enabled="1" method="Standard" siteId="{06219a4a-a835-44d5-afaf-3926343bfb89}" contentBits="0" removed="0"/>

</xml_diff>